<commit_message>
Blog 5 Pradheep edited
</commit_message>
<xml_diff>
--- a/blog Milestone 5.xlsx
+++ b/blog Milestone 5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\github\Library-Management-System-COEN-6312\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradheep\Desktop\Library-Management-System-COEN-6312\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B704836-F42E-45D3-82DB-935A63187C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EE874B-DD1F-491F-B98B-96B78011FAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="274">
   <si>
     <t>Team Members</t>
   </si>
@@ -840,6 +840,21 @@
   </si>
   <si>
     <t>Worked on ocl and class diagram</t>
+  </si>
+  <si>
+    <t>Diagram rework</t>
+  </si>
+  <si>
+    <t>Ocl object diagram reworks</t>
+  </si>
+  <si>
+    <t>Worked on Object Diagram rework formatting</t>
+  </si>
+  <si>
+    <t>Roprt compilation of deliverables 1,2 &amp; 3</t>
+  </si>
+  <si>
+    <t>Reoriented deliverable 5 draft with compiling and formatting</t>
   </si>
 </sst>
 </file>
@@ -1381,6 +1396,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1402,16 +1421,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF99FF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1710,10 +1730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S174"/>
+  <dimension ref="A1:S176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="N170" sqref="N170"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="O172" sqref="O172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1736,13 +1756,13 @@
     <row r="1" spans="1:19" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:19" ht="14.25" customHeight="1"/>
     <row r="3" spans="1:19" ht="16.5" customHeight="1">
-      <c r="H3" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="69"/>
-      <c r="S3" s="71" t="s">
+      <c r="H3" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="63"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="71"/>
+      <c r="S3" s="60" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1750,8 +1770,8 @@
       <c r="H4" s="1"/>
       <c r="I4" s="14"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="70"/>
-      <c r="S4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="S4" s="61"/>
     </row>
     <row r="5" spans="1:19" ht="14.25" customHeight="1">
       <c r="H5" s="2" t="s">
@@ -1763,8 +1783,8 @@
       <c r="J5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="70"/>
-      <c r="S5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="S5" s="61"/>
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1">
       <c r="H6" s="3" t="s">
@@ -1777,7 +1797,7 @@
         <v>7</v>
       </c>
       <c r="K6" s="16"/>
-      <c r="S6" s="72"/>
+      <c r="S6" s="61"/>
     </row>
     <row r="7" spans="1:19" ht="14.25" customHeight="1">
       <c r="H7" s="3" t="s">
@@ -1790,7 +1810,7 @@
         <v>10</v>
       </c>
       <c r="K7" s="16"/>
-      <c r="S7" s="72"/>
+      <c r="S7" s="61"/>
     </row>
     <row r="8" spans="1:19" ht="14.25" customHeight="1">
       <c r="H8" s="3" t="s">
@@ -1803,7 +1823,7 @@
         <v>11</v>
       </c>
       <c r="K8" s="16"/>
-      <c r="S8" s="72"/>
+      <c r="S8" s="61"/>
     </row>
     <row r="9" spans="1:19" ht="14.25" customHeight="1">
       <c r="H9" s="3" t="s">
@@ -1816,7 +1836,7 @@
         <v>15</v>
       </c>
       <c r="K9" s="16"/>
-      <c r="S9" s="72"/>
+      <c r="S9" s="61"/>
     </row>
     <row r="10" spans="1:19" ht="14.25" customHeight="1">
       <c r="H10" s="3" t="s">
@@ -1829,7 +1849,7 @@
         <v>18</v>
       </c>
       <c r="K10" s="16"/>
-      <c r="S10" s="72"/>
+      <c r="S10" s="61"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" customHeight="1">
       <c r="H11" s="4" t="s">
@@ -1842,7 +1862,7 @@
         <v>21</v>
       </c>
       <c r="K11" s="6"/>
-      <c r="S11" s="72"/>
+      <c r="S11" s="61"/>
     </row>
     <row r="12" spans="1:19" ht="14.25" customHeight="1">
       <c r="S12" t="s">
@@ -1856,41 +1876,41 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="65"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="67"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="68" t="s">
+      <c r="H15" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="69" t="s">
+      <c r="I15" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="68" t="s">
+      <c r="J15" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="68" t="s">
+      <c r="K15" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="63" t="s">
+      <c r="L15" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="M15" s="64"/>
-      <c r="N15" s="64"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="65"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="67"/>
       <c r="Q15" s="32"/>
       <c r="R15" s="33"/>
     </row>
     <row r="16" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A16" s="67"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="7" t="str">
         <f>$J$6</f>
         <v>Sai</v>
@@ -1915,10 +1935,10 @@
         <f>$J$11</f>
         <v>AS</v>
       </c>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
       <c r="L16" s="7" t="str">
         <f>$J$6</f>
         <v>Sai</v>
@@ -8968,34 +8988,34 @@
     </row>
     <row r="165" spans="1:18" ht="43.2">
       <c r="A165" s="40">
-        <v>45395</v>
-      </c>
-      <c r="B165" s="37">
-        <v>1</v>
-      </c>
+        <v>45394</v>
+      </c>
+      <c r="B165" s="37"/>
       <c r="C165" s="37"/>
       <c r="D165" s="37"/>
-      <c r="E165" s="37"/>
+      <c r="E165" s="37">
+        <v>1</v>
+      </c>
       <c r="F165" s="37"/>
       <c r="G165" s="37"/>
       <c r="H165" s="37" t="s">
         <v>195</v>
       </c>
       <c r="I165" s="43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J165" s="37" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="K165" s="37" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="L165" s="44">
-        <f t="shared" ref="L165:Q165" si="38">B165*$I165</f>
-        <v>3</v>
+        <f>S166</f>
+        <v>0</v>
       </c>
       <c r="M165" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="L165:Q165" si="38">C165*$I165</f>
         <v>0</v>
       </c>
       <c r="N165" s="44">
@@ -9003,8 +9023,7 @@
         <v>0</v>
       </c>
       <c r="O165" s="49">
-        <f t="shared" si="38"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P165" s="44">
         <f t="shared" si="38"/>
@@ -9016,54 +9035,38 @@
       </c>
       <c r="R165" s="28"/>
     </row>
-    <row r="166" spans="1:18" ht="28.8">
+    <row r="166" spans="1:18" ht="43.2">
       <c r="A166" s="40">
         <v>45395</v>
       </c>
-      <c r="B166" s="37"/>
+      <c r="B166" s="37">
+        <v>1</v>
+      </c>
       <c r="C166" s="37"/>
       <c r="D166" s="37"/>
       <c r="E166" s="37"/>
       <c r="F166" s="37"/>
-      <c r="G166" s="37">
-        <v>1</v>
-      </c>
+      <c r="G166" s="37"/>
       <c r="H166" s="37" t="s">
         <v>195</v>
       </c>
       <c r="I166" s="43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J166" s="37" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K166" s="37" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L166" s="44">
-        <f t="shared" ref="L166:Q169" si="39">B166*$I166</f>
-        <v>0</v>
-      </c>
-      <c r="M166" s="48">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="N166" s="44">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="O166" s="49">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="P166" s="44">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="Q166" s="44">
-        <f t="shared" si="39"/>
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="M166" s="48"/>
+      <c r="N166" s="44"/>
+      <c r="O166" s="49"/>
+      <c r="P166" s="44"/>
+      <c r="Q166" s="44"/>
       <c r="R166" s="28"/>
     </row>
     <row r="167" spans="1:18" ht="28.8">
@@ -9072,91 +9075,91 @@
       </c>
       <c r="B167" s="37"/>
       <c r="C167" s="37"/>
-      <c r="D167" s="37">
-        <v>1</v>
-      </c>
+      <c r="D167" s="37"/>
       <c r="E167" s="37"/>
       <c r="F167" s="37"/>
-      <c r="G167" s="37"/>
+      <c r="G167" s="37">
+        <v>1</v>
+      </c>
       <c r="H167" s="37" t="s">
         <v>195</v>
       </c>
       <c r="I167" s="43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J167" s="37" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="K167" s="37" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L167" s="44">
+        <f t="shared" ref="L167:Q171" si="39">B167*$I167</f>
         <v>0</v>
       </c>
       <c r="M167" s="48">
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="N167" s="44">
-        <v>3</v>
+        <f t="shared" si="39"/>
+        <v>0</v>
       </c>
       <c r="O167" s="49">
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="P167" s="44">
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Q167" s="44">
-        <v>0</v>
+        <f t="shared" si="39"/>
+        <v>1</v>
       </c>
       <c r="R167" s="28"/>
     </row>
-    <row r="168" spans="1:18" ht="43.2">
+    <row r="168" spans="1:18" ht="28.8">
       <c r="A168" s="40">
-        <v>45396</v>
+        <v>45395</v>
       </c>
       <c r="B168" s="37"/>
       <c r="C168" s="37"/>
-      <c r="D168" s="37"/>
+      <c r="D168" s="37">
+        <v>1</v>
+      </c>
       <c r="E168" s="37"/>
       <c r="F168" s="37"/>
-      <c r="G168" s="37">
-        <v>1</v>
-      </c>
+      <c r="G168" s="37"/>
       <c r="H168" s="37" t="s">
         <v>195</v>
       </c>
       <c r="I168" s="43">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="J168" s="37" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="K168" s="37" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="L168" s="44">
-        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="M168" s="48">
-        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="N168" s="44">
-        <f t="shared" si="39"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O168" s="49">
-        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="P168" s="44">
-        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Q168" s="44">
-        <f t="shared" si="39"/>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="R168" s="28"/>
     </row>
@@ -9164,169 +9167,253 @@
       <c r="A169" s="40">
         <v>45396</v>
       </c>
-      <c r="B169" s="37">
-        <v>1</v>
-      </c>
-      <c r="C169" s="37">
-        <v>1</v>
-      </c>
-      <c r="D169" s="37">
-        <v>1</v>
-      </c>
+      <c r="B169" s="37"/>
+      <c r="C169" s="37"/>
+      <c r="D169" s="37"/>
       <c r="E169" s="37">
         <v>1</v>
       </c>
-      <c r="F169" s="37">
-        <v>1</v>
-      </c>
-      <c r="G169" s="37">
-        <v>1</v>
-      </c>
+      <c r="F169" s="37"/>
+      <c r="G169" s="37"/>
       <c r="H169" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="I169" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="J169" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="K169" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="L169" s="44"/>
+      <c r="M169" s="48"/>
+      <c r="N169" s="44"/>
+      <c r="O169" s="49">
+        <v>2.5</v>
+      </c>
+      <c r="P169" s="44"/>
+      <c r="Q169" s="44"/>
+      <c r="R169" s="28"/>
+    </row>
+    <row r="170" spans="1:18" ht="43.2">
+      <c r="A170" s="40">
+        <v>45396</v>
+      </c>
+      <c r="B170" s="37"/>
+      <c r="C170" s="37"/>
+      <c r="D170" s="37"/>
+      <c r="E170" s="37"/>
+      <c r="F170" s="37"/>
+      <c r="G170" s="37">
+        <v>1</v>
+      </c>
+      <c r="H170" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="I170" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="J170" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="K170" s="37" t="s">
+        <v>262</v>
+      </c>
+      <c r="L170" s="44">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="M170" s="48">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="N170" s="44">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="O170" s="49">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="P170" s="44">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="Q170" s="44">
+        <f t="shared" si="39"/>
+        <v>2.5</v>
+      </c>
+      <c r="R170" s="28"/>
+    </row>
+    <row r="171" spans="1:18" ht="28.8">
+      <c r="A171" s="40">
+        <v>45396</v>
+      </c>
+      <c r="B171" s="37">
+        <v>1</v>
+      </c>
+      <c r="C171" s="37">
+        <v>1</v>
+      </c>
+      <c r="D171" s="37">
+        <v>1</v>
+      </c>
+      <c r="E171" s="37">
+        <v>1</v>
+      </c>
+      <c r="F171" s="37">
+        <v>1</v>
+      </c>
+      <c r="G171" s="37">
+        <v>1</v>
+      </c>
+      <c r="H171" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="I169" s="43">
-        <v>1</v>
-      </c>
-      <c r="J169" s="37" t="s">
+      <c r="I171" s="43">
+        <v>1</v>
+      </c>
+      <c r="J171" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="K169" s="37" t="s">
+      <c r="K171" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="L169" s="44">
+      <c r="L171" s="44">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="M169" s="48">
+      <c r="M171" s="48">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="N169" s="44">
+      <c r="N171" s="44">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="O169" s="49">
+      <c r="O171" s="49">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="P169" s="44">
+      <c r="P171" s="44">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="Q169" s="44">
+      <c r="Q171" s="44">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="R169" s="28"/>
-    </row>
-    <row r="170" spans="1:18" ht="14.25" customHeight="1">
-      <c r="A170" s="13"/>
-      <c r="H170" s="27"/>
-      <c r="K170" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="L170" s="47">
-        <f t="shared" ref="L170:Q170" si="40">SUM(L165:L169)</f>
-        <v>4</v>
-      </c>
-      <c r="M170" s="50">
-        <f t="shared" si="40"/>
-        <v>1</v>
-      </c>
-      <c r="N170" s="47">
-        <f t="shared" si="40"/>
-        <v>4</v>
-      </c>
-      <c r="O170" s="51">
-        <f t="shared" si="40"/>
-        <v>1</v>
-      </c>
-      <c r="P170" s="46">
-        <f t="shared" si="40"/>
-        <v>1</v>
-      </c>
-      <c r="Q170" s="46">
-        <f t="shared" si="40"/>
-        <v>4.5</v>
-      </c>
-      <c r="R170">
-        <f>SUM(L170:Q170)</f>
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="171" spans="1:18" ht="14.25" customHeight="1">
-      <c r="A171" s="13"/>
-      <c r="K171" s="50" t="s">
-        <v>264</v>
-      </c>
-      <c r="L171" s="47"/>
-      <c r="M171" s="50"/>
-      <c r="N171" s="47"/>
-      <c r="O171" s="51"/>
-      <c r="P171" s="46"/>
-      <c r="Q171" s="46"/>
+      <c r="R171" s="28"/>
     </row>
     <row r="172" spans="1:18" ht="14.25" customHeight="1">
       <c r="A172" s="13"/>
-      <c r="L172" s="52"/>
-      <c r="N172" s="53"/>
-      <c r="P172" s="54"/>
-      <c r="Q172" s="28"/>
+      <c r="H172" s="27"/>
+      <c r="K172" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="L172" s="47">
+        <f>SUM(L165:L171)</f>
+        <v>4</v>
+      </c>
+      <c r="M172" s="50">
+        <f>SUM(M165:M171)</f>
+        <v>1</v>
+      </c>
+      <c r="N172" s="47">
+        <f>SUM(N165:N171)</f>
+        <v>4</v>
+      </c>
+      <c r="O172" s="51">
+        <f>SUM(O165:O171)</f>
+        <v>5.5</v>
+      </c>
+      <c r="P172" s="46">
+        <f>SUM(P165:P171)</f>
+        <v>1</v>
+      </c>
+      <c r="Q172" s="46">
+        <f>SUM(Q165:Q171)</f>
+        <v>4.5</v>
+      </c>
+      <c r="R172">
+        <f>SUM(L172:Q172)</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="173" spans="1:18" ht="14.25" customHeight="1">
       <c r="A173" s="13"/>
-      <c r="K173" s="55" t="s">
+      <c r="K173" s="50" t="s">
+        <v>264</v>
+      </c>
+      <c r="L173" s="47"/>
+      <c r="M173" s="50"/>
+      <c r="N173" s="47"/>
+      <c r="O173" s="51"/>
+      <c r="P173" s="46"/>
+      <c r="Q173" s="46"/>
+    </row>
+    <row r="174" spans="1:18" ht="14.25" customHeight="1">
+      <c r="A174" s="13"/>
+      <c r="L174" s="52"/>
+      <c r="N174" s="53"/>
+      <c r="P174" s="54"/>
+      <c r="Q174" s="28"/>
+    </row>
+    <row r="175" spans="1:18" ht="14.25" customHeight="1">
+      <c r="A175" s="13"/>
+      <c r="K175" s="55" t="s">
         <v>265</v>
       </c>
-      <c r="L173" s="53">
-        <f t="shared" ref="L173:Q173" si="41">L34+L90+L130+L162+L170</f>
+      <c r="L175" s="53">
+        <f>L34+L90+L130+L162+L172</f>
         <v>87.5</v>
       </c>
-      <c r="M173">
-        <f t="shared" si="41"/>
+      <c r="M175">
+        <f>M34+M90+M130+M162+M172</f>
         <v>84.5</v>
       </c>
-      <c r="N173" s="53">
-        <f t="shared" si="41"/>
+      <c r="N175" s="53">
+        <f>N34+N90+N130+N162+N172</f>
         <v>87</v>
       </c>
-      <c r="O173">
-        <f t="shared" si="41"/>
-        <v>86.5</v>
-      </c>
-      <c r="P173" s="56">
-        <f t="shared" si="41"/>
+      <c r="O175">
+        <f>O34+O90+O130+O162+O172</f>
+        <v>91</v>
+      </c>
+      <c r="P175" s="56">
+        <f>P34+P90+P130+P162+P172</f>
         <v>86</v>
       </c>
-      <c r="Q173" s="28">
-        <f t="shared" si="41"/>
+      <c r="Q175" s="28">
+        <f>Q34+Q90+Q130+Q162+Q172</f>
         <v>87</v>
       </c>
     </row>
-    <row r="174" spans="1:18" ht="14.25" customHeight="1">
-      <c r="A174" s="41"/>
-      <c r="B174" s="42"/>
-      <c r="C174" s="42"/>
-      <c r="D174" s="42"/>
-      <c r="E174" s="42"/>
-      <c r="F174" s="42"/>
-      <c r="G174" s="42"/>
-      <c r="H174" s="42"/>
-      <c r="I174" s="42"/>
-      <c r="J174" s="42"/>
-      <c r="K174" s="57" t="s">
+    <row r="176" spans="1:18" ht="14.25" customHeight="1">
+      <c r="A176" s="41"/>
+      <c r="B176" s="42"/>
+      <c r="C176" s="42"/>
+      <c r="D176" s="42"/>
+      <c r="E176" s="42"/>
+      <c r="F176" s="42"/>
+      <c r="G176" s="42"/>
+      <c r="H176" s="42"/>
+      <c r="I176" s="42"/>
+      <c r="J176" s="42"/>
+      <c r="K176" s="57" t="s">
         <v>266</v>
       </c>
-      <c r="L174" s="58"/>
-      <c r="M174" s="42"/>
-      <c r="N174" s="59"/>
-      <c r="O174" s="42"/>
-      <c r="P174" s="59"/>
-      <c r="Q174" s="34"/>
-      <c r="R174">
-        <f>SUM(L173:Q173)</f>
-        <v>518.5</v>
+      <c r="L176" s="58"/>
+      <c r="M176" s="42"/>
+      <c r="N176" s="59"/>
+      <c r="O176" s="42"/>
+      <c r="P176" s="59"/>
+      <c r="Q176" s="34"/>
+      <c r="R176">
+        <f>SUM(L175:Q175)</f>
+        <v>523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>